<commit_message>
Actualizar archivo de preguntas en formato Excel
</commit_message>
<xml_diff>
--- a/Preguntas.xlsx
+++ b/Preguntas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dairon Alonso\Desktop\App Streamlit\App-Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A641007-5532-4D77-868C-389FDD3B30EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A32BB35-9ABB-40F2-912D-D58A69DCBED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,9 +553,6 @@
     <t>120W.; 68W.; 80W.; 90W.</t>
   </si>
   <si>
-    <t>15.; 10.; 8.; 12.</t>
-  </si>
-  <si>
     <t>Sony LYTIA 700C.; Sony LYTIA 600C.; Sony LYTIA 750C; Sony LYTIA 660C</t>
   </si>
   <si>
@@ -838,9 +835,6 @@
     <t>90W.</t>
   </si>
   <si>
-    <t>12.</t>
-  </si>
-  <si>
     <t>Sony LYTIA 600C.</t>
   </si>
   <si>
@@ -905,6 +899,12 @@
   </si>
   <si>
     <t>5200 mAh</t>
+  </si>
+  <si>
+    <t>12 gb</t>
+  </si>
+  <si>
+    <t>15 gb;10 gb;8 gb;12 gb</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1268,8 @@
   </sheetPr>
   <dimension ref="A1:D551"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1303,7 @@
         <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1331,7 +1331,7 @@
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1373,7 +1373,7 @@
         <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
         <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>139</v>
       </c>
       <c r="D39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>147</v>
       </c>
       <c r="D47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1961,7 +1961,7 @@
         <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>160</v>
       </c>
       <c r="D60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>163</v>
       </c>
       <c r="D63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>169</v>
       </c>
       <c r="D69" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
         <v>170</v>
       </c>
       <c r="D70" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>173</v>
       </c>
       <c r="D73" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>174</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
         <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>176</v>
       </c>
       <c r="D76" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2350,10 +2350,10 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>177</v>
+        <v>294</v>
       </c>
       <c r="D77" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2364,10 +2364,10 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D78" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2378,10 +2378,10 @@
         <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D79" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2392,10 +2392,10 @@
         <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D80" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,10 +2406,10 @@
         <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D81" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2420,10 +2420,10 @@
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D82" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2434,10 +2434,10 @@
         <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D83" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2448,10 +2448,10 @@
         <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D84" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,10 +2462,10 @@
         <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D85" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,10 +2476,10 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2490,10 +2490,10 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D87" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,10 +2504,10 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D88" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2518,10 +2518,10 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D89" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,10 +2532,10 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D90" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2546,10 +2546,10 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D91" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2560,10 +2560,10 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D92" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,10 +2574,10 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D93" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,10 +2588,10 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D94" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,10 +2602,10 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D95" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D96" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2630,10 +2630,10 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,10 +2644,10 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D98" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2658,10 +2658,10 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D99" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2672,10 +2672,10 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D100" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2686,10 +2686,10 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D101" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mejorar estilos de presentación y manejo de opciones en el archivo de preguntas
</commit_message>
<xml_diff>
--- a/Preguntas.xlsx
+++ b/Preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dairon Alonso\Desktop\App Streamlit\App-Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A32BB35-9ABB-40F2-912D-D58A69DCBED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF83BAD3-DCC0-4225-AA6E-6D26134FB2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,9 +577,6 @@
     <t>Startac 01.; Razr V3.; Moto One.; DynaTAC 8000x</t>
   </si>
   <si>
-    <t>1.; 2.; 4.; 3.</t>
-  </si>
-  <si>
     <t>Graba solo la Cámara posterior a 4k.; Falso, graba en Full HD+ ambas cámaras.; Ambas cámaras (Posterior y frontal) graba a 4k.; Ambas cámaras (Posterior y frontal) graba: Super HD.</t>
   </si>
   <si>
@@ -856,9 +853,6 @@
     <t>DynaTAC 8000x</t>
   </si>
   <si>
-    <t>3.</t>
-  </si>
-  <si>
     <t>Ambas cámaras (Posterior y frontal) graba a 4k.</t>
   </si>
   <si>
@@ -905,6 +899,12 @@
   </si>
   <si>
     <t>15 gb;10 gb;8 gb;12 gb</t>
+  </si>
+  <si>
+    <t>Uno ; Dos ; Cuatro ; Tres</t>
+  </si>
+  <si>
+    <t>Tres</t>
   </si>
 </sst>
 </file>
@@ -1268,8 +1268,8 @@
   </sheetPr>
   <dimension ref="A1:D551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1303,7 @@
         <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1331,7 +1331,7 @@
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1373,7 +1373,7 @@
         <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
         <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>139</v>
       </c>
       <c r="D39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>147</v>
       </c>
       <c r="D47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1961,7 +1961,7 @@
         <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>160</v>
       </c>
       <c r="D60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>163</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>169</v>
       </c>
       <c r="D69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
         <v>170</v>
       </c>
       <c r="D70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>173</v>
       </c>
       <c r="D73" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>174</v>
       </c>
       <c r="D74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
         <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>176</v>
       </c>
       <c r="D76" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2350,10 +2350,10 @@
         <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D77" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>177</v>
       </c>
       <c r="D78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>178</v>
       </c>
       <c r="D79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>179</v>
       </c>
       <c r="D80" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>180</v>
       </c>
       <c r="D81" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
         <v>181</v>
       </c>
       <c r="D82" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>182</v>
       </c>
       <c r="D83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,7 +2451,7 @@
         <v>183</v>
       </c>
       <c r="D84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>184</v>
       </c>
       <c r="D85" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,10 +2476,10 @@
         <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>185</v>
+        <v>293</v>
       </c>
       <c r="D86" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2490,10 +2490,10 @@
         <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D87" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,10 +2504,10 @@
         <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D88" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2518,10 +2518,10 @@
         <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D89" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,10 +2532,10 @@
         <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D90" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2546,10 +2546,10 @@
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D91" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2560,10 +2560,10 @@
         <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D92" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,10 +2574,10 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D93" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,10 +2588,10 @@
         <v>96</v>
       </c>
       <c r="C94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D94" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,10 +2602,10 @@
         <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D96" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2630,10 +2630,10 @@
         <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D97" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,10 +2644,10 @@
         <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D98" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2658,10 +2658,10 @@
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D99" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2672,10 +2672,10 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D100" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2686,10 +2686,10 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D101" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>